<commit_message>
add placeholder back into calendar date so swagger works correctly
</commit_message>
<xml_diff>
--- a/EdFiXLearningModality-ProgramAndCalendarMethod/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
+++ b/EdFiXLearningModality-ProgramAndCalendarMethod/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
@@ -376,7 +376,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ed-Fi Handbook"/>
-  <dimension ref="A1:G960"/>
+  <dimension ref="A1:G961"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -25253,21 +25253,45 @@
         <v/>
       </c>
       <c r="B956" t="str">
+        <v>PlaceHolderProp</v>
+      </c>
+      <c r="C956" t="str">
+        <v>Dummy Prop to overcome a bug</v>
+      </c>
+      <c r="D956" t="str">
+        <v>Boolean</v>
+      </c>
+      <c r="E956" t="str">
+        <v/>
+      </c>
+      <c r="F956" t="str">
+        <v/>
+      </c>
+      <c r="G956" t="str" xml:space="preserve">
+        <v xml:space="preserve">Used By:
+CalendarDate.PlaceHolderProp (as optional)</v>
+      </c>
+    </row>
+    <row r="957" xml:space="preserve">
+      <c r="A957" t="str">
+        <v/>
+      </c>
+      <c r="B957" t="str">
         <v>LearningModality (EdFiXLearningModality)</v>
       </c>
-      <c r="C956" t="str">
+      <c r="C957" t="str">
         <v>Captures key aspects of the student learning modality.</v>
       </c>
-      <c r="D956" t="str">
+      <c r="D957" t="str">
         <v>Composite Part</v>
       </c>
-      <c r="E956" t="str">
-        <v/>
-      </c>
-      <c r="F956" t="str">
-        <v/>
-      </c>
-      <c r="G956" t="str" xml:space="preserve">
+      <c r="E957" t="str">
+        <v/>
+      </c>
+      <c r="F957" t="str">
+        <v/>
+      </c>
+      <c r="G957" t="str" xml:space="preserve">
         <v xml:space="preserve">Contains:
 ModalityTime (required)
 ModalityTimeType (required)
@@ -25277,26 +25301,26 @@
 Program.LearningModality (as optional collection)</v>
       </c>
     </row>
-    <row r="957" xml:space="preserve">
-      <c r="A957" t="str">
-        <v/>
-      </c>
-      <c r="B957" t="str">
+    <row r="958" xml:space="preserve">
+      <c r="A958" t="str">
+        <v/>
+      </c>
+      <c r="B958" t="str">
         <v>ProgramLearningModalityType (EdFiXLearningModality)</v>
       </c>
-      <c r="C957" t="str">
+      <c r="C958" t="str">
         <v>A collection of Learning Modalities associated with a Program that may be tied to Calendar Dates.</v>
       </c>
-      <c r="D957" t="str">
+      <c r="D958" t="str">
         <v>Composite Part</v>
       </c>
-      <c r="E957" t="str">
-        <v/>
-      </c>
-      <c r="F957" t="str">
-        <v/>
-      </c>
-      <c r="G957" t="str" xml:space="preserve">
+      <c r="E958" t="str">
+        <v/>
+      </c>
+      <c r="F958" t="str">
+        <v/>
+      </c>
+      <c r="G958" t="str" xml:space="preserve">
         <v xml:space="preserve">Contains:
 LearningModality (optional collection)
 Program (identity)
@@ -25304,53 +25328,29 @@
 CalendarDate.ProgramLearningModalityType (as optional collection)</v>
       </c>
     </row>
-    <row r="958" xml:space="preserve">
-      <c r="A958" t="str">
-        <v/>
-      </c>
-      <c r="B958" t="str">
+    <row r="959" xml:space="preserve">
+      <c r="A959" t="str">
+        <v/>
+      </c>
+      <c r="B959" t="str">
         <v>ModalityTime</v>
       </c>
-      <c r="C958" t="str">
+      <c r="C959" t="str">
         <v>The duration the student engaged via the modality.</v>
       </c>
-      <c r="D958" t="str">
+      <c r="D959" t="str">
         <v>Number</v>
       </c>
-      <c r="E958" t="str" xml:space="preserve">
+      <c r="E959" t="str" xml:space="preserve">
         <v xml:space="preserve">total digits: 8
 decimal places: 2
 min value: 0</v>
       </c>
-      <c r="F958" t="str">
-        <v/>
-      </c>
-      <c r="G958" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="959" xml:space="preserve">
-      <c r="A959" t="str">
-        <v/>
-      </c>
-      <c r="B959" t="str">
-        <v>ModalityTimeType (EdFiXLearningModality)</v>
-      </c>
-      <c r="C959" t="str">
-        <v>The units or time dimension for hte duration.</v>
-      </c>
-      <c r="D959" t="str">
-        <v>Descriptor</v>
-      </c>
-      <c r="E959" t="str">
-        <v/>
-      </c>
       <c r="F959" t="str">
         <v/>
       </c>
-      <c r="G959" t="str" xml:space="preserve">
-        <v xml:space="preserve">Used By:
-LearningModality.ModalityTimeType (as required)</v>
+      <c r="G959" t="str">
+        <v/>
       </c>
     </row>
     <row r="960" xml:space="preserve">
@@ -25358,10 +25358,10 @@
         <v/>
       </c>
       <c r="B960" t="str">
-        <v>ModalityType (EdFiXLearningModality)</v>
+        <v>ModalityTimeType (EdFiXLearningModality)</v>
       </c>
       <c r="C960" t="str">
-        <v>The method by which the student is engaging in instruction.</v>
+        <v>The units or time dimension for hte duration.</v>
       </c>
       <c r="D960" t="str">
         <v>Descriptor</v>
@@ -25373,6 +25373,30 @@
         <v/>
       </c>
       <c r="G960" t="str" xml:space="preserve">
+        <v xml:space="preserve">Used By:
+LearningModality.ModalityTimeType (as required)</v>
+      </c>
+    </row>
+    <row r="961" xml:space="preserve">
+      <c r="A961" t="str">
+        <v/>
+      </c>
+      <c r="B961" t="str">
+        <v>ModalityType (EdFiXLearningModality)</v>
+      </c>
+      <c r="C961" t="str">
+        <v>The method by which the student is engaging in instruction.</v>
+      </c>
+      <c r="D961" t="str">
+        <v>Descriptor</v>
+      </c>
+      <c r="E961" t="str">
+        <v/>
+      </c>
+      <c r="F961" t="str">
+        <v/>
+      </c>
+      <c r="G961" t="str" xml:space="preserve">
         <v xml:space="preserve">Used By:
 LearningModality.ModalityType (as identity)</v>
       </c>

</xml_diff>